<commit_message>
1. Modified the forest plot to plot standardized mean differences between treatment arms.
</commit_message>
<xml_diff>
--- a/data/rct_LVEF.xlsx
+++ b/data/rct_LVEF.xlsx
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
-    <t>Study</t>
-  </si>
-  <si>
     <t>n</t>
   </si>
   <si>
@@ -93,6 +90,9 @@
   </si>
   <si>
     <t>LVEF (%)</t>
+  </si>
+  <si>
+    <t>study</t>
   </si>
 </sst>
 </file>
@@ -421,9 +421,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -434,54 +432,54 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>251</v>
       </c>
       <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F2">
         <v>126</v>
@@ -504,19 +502,19 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>301</v>
       </c>
       <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3">
         <v>151</v>
@@ -539,19 +537,19 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4">
         <v>401</v>
       </c>
       <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4">
         <v>203</v>
@@ -574,19 +572,19 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5">
         <v>260</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
         <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
       </c>
       <c r="F5">
         <v>127</v>

</xml_diff>

<commit_message>
1. Each study has been renamed to match the ones in the grant proposal. 2. Made the plot more compact.
</commit_message>
<xml_diff>
--- a/data/rct_LVEF.xlsx
+++ b/data/rct_LVEF.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
-  <si>
-    <t>n</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>n_ctrl</t>
   </si>
@@ -93,6 +90,21 @@
   </si>
   <si>
     <t>study</t>
+  </si>
+  <si>
+    <t>CTSN Severe MR</t>
+  </si>
+  <si>
+    <t>CTSN Moderate MR</t>
+  </si>
+  <si>
+    <t>CTSN TR Trial</t>
+  </si>
+  <si>
+    <t>CTSN AF Trial</t>
+  </si>
+  <si>
+    <t>author_year</t>
   </si>
 </sst>
 </file>
@@ -421,65 +433,68 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" customWidth="1"/>
     <col min="4" max="5" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>251</v>
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
       </c>
       <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2">
         <v>126</v>
@@ -502,19 +517,19 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3">
-        <v>301</v>
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
       </c>
       <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3">
         <v>151</v>
@@ -537,19 +552,19 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="B4">
-        <v>401</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4">
         <v>203</v>
@@ -572,19 +587,19 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
         <v>19</v>
       </c>
-      <c r="B5">
-        <v>260</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
       </c>
       <c r="F5">
         <v>127</v>

</xml_diff>